<commit_message>
setting binary path in class file
</commit_message>
<xml_diff>
--- a/src/com/uat/xls/Crendiantial_User.xlsx
+++ b/src/com/uat/xls/Crendiantial_User.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="7680"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>Username</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>Test Mnagement</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +686,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>